<commit_message>
fixed up some bugs
</commit_message>
<xml_diff>
--- a/T3Dir/JoeysStaff.xlsx
+++ b/T3Dir/JoeysStaff.xlsx
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>44.25</v>
       </c>
     </row>
     <row r="4">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>